<commit_message>
Worked on the UML-diagrams, they're almost done. Nothing big left to do.
Signed-off-by: Noa <noa@stojanovic.ch>
</commit_message>
<xml_diff>
--- a/UML-Diagramme(not finished).xlsx
+++ b/UML-Diagramme(not finished).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noa\Documents\Schule\MA_NoaHerzog_19Md\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EC9C719-9EA1-4FCB-9F6F-00BEBA8218E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C732DC03-B857-42A7-9AC8-00F9E6AEBB08}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11040" xr2:uid="{7C2311B0-2396-43ED-8785-5D59890FFFB1}"/>
   </bookViews>
@@ -94,10 +94,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Grafik 1" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image001.png">
+        <xdr:cNvPr id="10" name="Grafik 9" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image001.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AEB08FC-6BAF-4843-A0F1-2FE038A5D2CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E206398-612F-4730-9E82-6E15DF5F36B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -149,16 +149,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>557213</xdr:colOff>
       <xdr:row>101</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image002.png">
+        <xdr:cNvPr id="11" name="Grafik 10" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image002.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FA681B7-F81D-4880-89A1-E81C9E2DF39F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E71AF87-EAC2-41DC-86B1-295E30CF2975}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -182,7 +182,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="36580763" y="0"/>
-          <a:ext cx="9144000" cy="18288000"/>
+          <a:ext cx="9696450" cy="18288000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -216,10 +216,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Grafik 3" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image003.png">
+        <xdr:cNvPr id="12" name="Grafik 11" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image003.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C21E7BC6-B4AA-4015-8E3F-946B4D051D64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37F34A6F-033C-47D6-99B8-E882A0583B51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -271,16 +271,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>557213</xdr:colOff>
       <xdr:row>202</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Grafik 4" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image004.png">
+        <xdr:cNvPr id="13" name="Grafik 12" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image004.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B1BA2EF-F41B-477C-86FE-941E2E92900F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7D71A35-D160-4608-A4F2-016189EF4A88}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -304,7 +304,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="36580763" y="18278475"/>
-          <a:ext cx="9144000" cy="18288000"/>
+          <a:ext cx="9696450" cy="18288000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -338,10 +338,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Grafik 5" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image005.png">
+        <xdr:cNvPr id="14" name="Grafik 13" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image005.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{032781DA-8092-4842-A114-613B42D0644A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E639F673-F4A8-45A8-8B57-45BA1B0A981E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -393,16 +393,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>557213</xdr:colOff>
       <xdr:row>303</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Grafik 6" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image006.png">
+        <xdr:cNvPr id="15" name="Grafik 14" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image006.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F7D68A9-E60A-4C47-81B6-A64ACD8187C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6647F8D-997B-44D5-B01A-11261FFF4E26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -426,7 +426,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="36580763" y="36556950"/>
-          <a:ext cx="9144000" cy="18288000"/>
+          <a:ext cx="9696450" cy="18288000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -460,10 +460,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Grafik 7" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image007.png">
+        <xdr:cNvPr id="16" name="Grafik 15" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image007.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0765BC9F-1513-4BFC-87F5-00B2949359A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FEBB9E-C93B-4F48-9237-10F75067EE7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -515,16 +515,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>557213</xdr:colOff>
       <xdr:row>351</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Grafik 8" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image008.png">
+        <xdr:cNvPr id="17" name="Grafik 16" descr="C:\Users\Noa\AppData\Local\Packages\Microsoft.Office.OneNote_8wekyb3d8bbwe\TempState\msohtmlclip\clip_image008.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB304CEF-1E4F-4F68-A783-A2E0E9130CFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA776015-B4DE-4DDE-B4A7-E4D399A2C298}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -548,7 +548,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="36580763" y="54835425"/>
-          <a:ext cx="9144000" cy="8743950"/>
+          <a:ext cx="9696450" cy="8743950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E229B84-5D2B-47FA-9161-1EE6E814A016}">
   <dimension ref="A1:A350"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="1" sqref="A1:A350 C11"/>
+    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>